<commit_message>
Add authors to relatorio
</commit_message>
<xml_diff>
--- a/t4/INF1413_HGLK_Trab4.Relatório_20170621.xlsx
+++ b/t4/INF1413_HGLK_Trab4.Relatório_20170621.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>Data</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>Estudei o enunciado do trabalho</t>
+  </si>
+  <si>
+    <t>Autores:</t>
+  </si>
+  <si>
+    <t>Hugo Grochau</t>
+  </si>
+  <si>
+    <t>Leonardo Kaplan</t>
   </si>
 </sst>
 </file>
@@ -109,7 +118,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="164" formatCode="d/m/yy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -153,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -221,11 +230,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -239,11 +263,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F12"/>
+  <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,75 +603,52 @@
   <sheetData>
     <row r="2" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="5">
-        <v>42896</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="5">
-        <v>42897</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
-        <v>42901</v>
+        <v>42896</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>11</v>
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
-        <v>42902</v>
+        <v>42897</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>8</v>
@@ -652,16 +656,16 @@
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>12</v>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
-        <v>42539</v>
+        <v>42901</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -669,95 +673,129 @@
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
-        <v>42905</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>24</v>
+        <v>42902</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>16</v>
+      <c r="B9" s="5">
+        <v>42539</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
+        <v>42905</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="5">
-        <v>42542</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <v>42542</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>